<commit_message>
inicia datawise seeders, y parte de front datawise view
</commit_message>
<xml_diff>
--- a/backend/data/DataWise_data.xlsx
+++ b/backend/data/DataWise_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/Google Drive/FINAC/Oahub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA50C04-D1DC-BA4D-B2BD-4991551A1B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4669504-C655-384D-9EB6-0C5BC14E8F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22480" yWindow="2580" windowWidth="27200" windowHeight="15540" firstSheet="11" activeTab="18" xr2:uid="{44AB9135-6F36-43A2-8618-128F6D28EF18}"/>
+    <workbookView xWindow="17360" yWindow="7240" windowWidth="10000" windowHeight="13140" firstSheet="9" activeTab="8" xr2:uid="{44AB9135-6F36-43A2-8618-128F6D28EF18}"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="18" r:id="rId1"/>
@@ -18,10 +18,10 @@
     <sheet name="Escuelas" sheetId="15" r:id="rId3"/>
     <sheet name="Areas" sheetId="6" r:id="rId4"/>
     <sheet name="Temas" sheetId="13" r:id="rId5"/>
-    <sheet name="Grados" sheetId="16" r:id="rId6"/>
+    <sheet name="Grades" sheetId="16" r:id="rId6"/>
     <sheet name="Secciones" sheetId="19" r:id="rId7"/>
     <sheet name="Materias" sheetId="4" r:id="rId8"/>
-    <sheet name="Items" sheetId="10" r:id="rId9"/>
+    <sheet name="Herramientas" sheetId="10" r:id="rId9"/>
     <sheet name="Académicos" sheetId="1" r:id="rId10"/>
     <sheet name="Académico-materia_grado_sección" sheetId="5" r:id="rId11"/>
     <sheet name="Items_temas" sheetId="14" r:id="rId12"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="128">
   <si>
     <t>Académico_1</t>
   </si>
@@ -285,13 +285,166 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>name_es</t>
+  </si>
+  <si>
+    <t>name_en</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Unit_1</t>
+  </si>
+  <si>
+    <t>Unit_2</t>
+  </si>
+  <si>
+    <t>Unit_3</t>
+  </si>
+  <si>
+    <t>Unit_4</t>
+  </si>
+  <si>
+    <t>Unit_5</t>
+  </si>
+  <si>
+    <t>Escuela_4</t>
+  </si>
+  <si>
+    <t>School_1</t>
+  </si>
+  <si>
+    <t>School_2</t>
+  </si>
+  <si>
+    <t>School_3</t>
+  </si>
+  <si>
+    <t>School_4</t>
+  </si>
+  <si>
+    <t>Area_4</t>
+  </si>
+  <si>
+    <t>Area_5</t>
+  </si>
+  <si>
+    <t>Topic_1</t>
+  </si>
+  <si>
+    <t>Topic_2</t>
+  </si>
+  <si>
+    <t>Topic_3</t>
+  </si>
+  <si>
+    <t>Grade_1</t>
+  </si>
+  <si>
+    <t>Grade_2</t>
+  </si>
+  <si>
+    <t>Grade_3</t>
+  </si>
+  <si>
+    <t>Grade_4</t>
+  </si>
+  <si>
+    <t>Subject_1</t>
+  </si>
+  <si>
+    <t>Subject_2</t>
+  </si>
+  <si>
+    <t>Subject_3</t>
+  </si>
+  <si>
+    <t>Subject_4</t>
+  </si>
+  <si>
+    <t>Subject_5</t>
+  </si>
+  <si>
+    <t>Subject_6</t>
+  </si>
+  <si>
+    <t>Herramienta_1</t>
+  </si>
+  <si>
+    <t>Herramienta_2</t>
+  </si>
+  <si>
+    <t>Herramienta_3</t>
+  </si>
+  <si>
+    <t>Herramienta_4</t>
+  </si>
+  <si>
+    <t>Herramienta_5</t>
+  </si>
+  <si>
+    <t>Herramienta_6</t>
+  </si>
+  <si>
+    <t>Herramienta_7</t>
+  </si>
+  <si>
+    <t>Herramienta_8</t>
+  </si>
+  <si>
+    <t>Herramienta_9</t>
+  </si>
+  <si>
+    <t>Herramienta_10</t>
+  </si>
+  <si>
+    <t>Herramienta_11</t>
+  </si>
+  <si>
+    <t>Tool_1</t>
+  </si>
+  <si>
+    <t>Tool_2</t>
+  </si>
+  <si>
+    <t>Tool_3</t>
+  </si>
+  <si>
+    <t>Tool_4</t>
+  </si>
+  <si>
+    <t>Tool_5</t>
+  </si>
+  <si>
+    <t>Tool_6</t>
+  </si>
+  <si>
+    <t>Tool_7</t>
+  </si>
+  <si>
+    <t>Tool_8</t>
+  </si>
+  <si>
+    <t>Tool_9</t>
+  </si>
+  <si>
+    <t>Tool_10</t>
+  </si>
+  <si>
+    <t>Tool_11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,6 +454,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -328,7 +488,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AAD4E0-7EF2-134F-A9A0-0DE4803FFE3F}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -654,19 +814,36 @@
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1671,7 +1848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A9B27E-E1A6-415D-BD06-C8E0BDBAB3C3}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -1725,37 +1902,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392E348C-14A0-4F43-A248-CDFC09B373D7}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>73</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1766,160 +1966,275 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AB04F78-20E6-F04A-A4CC-59D1F05547D5}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A6C17D-B7EE-4711-94AF-14518E98A3F5}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>29</v>
       </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13288D26-1715-43A0-91D2-35D274861EBC}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>64</v>
       </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20AB50A6-431D-184F-94EE-B7A1F485BCE2}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB9281A-B767-3444-947F-A4BE344A4582}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1931,112 +2246,183 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81DEEA14-CFFA-4C60-B0C0-920B78619759}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>24</v>
       </c>
+      <c r="B7" t="s">
+        <v>105</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F276F6-33EA-40C9-B929-6DEBAF0DDEAA}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="B6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="B8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>115</v>
+      </c>
+      <c r="B11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambio en cargue de grades y schools
</commit_message>
<xml_diff>
--- a/backend/data/DataWise_data.xlsx
+++ b/backend/data/DataWise_data.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/Documents/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6797A1AA-4D0F-ED4C-B0E1-88615069592A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9A1D19-83AB-BB49-9F8F-3C487995D0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22240" yWindow="12160" windowWidth="21340" windowHeight="12740" activeTab="6" xr2:uid="{44AB9135-6F36-43A2-8618-128F6D28EF18}"/>
+    <workbookView xWindow="1020" yWindow="4600" windowWidth="21340" windowHeight="12740" firstSheet="2" activeTab="9" xr2:uid="{44AB9135-6F36-43A2-8618-128F6D28EF18}"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="18" r:id="rId1"/>
     <sheet name="UnidadesServicio" sheetId="17" r:id="rId2"/>
     <sheet name="Escuelas" sheetId="15" r:id="rId3"/>
-    <sheet name="Areas" sheetId="6" r:id="rId4"/>
-    <sheet name="Temas" sheetId="13" r:id="rId5"/>
-    <sheet name="Grades" sheetId="16" r:id="rId6"/>
-    <sheet name="Materias" sheetId="4" r:id="rId7"/>
-    <sheet name="Secciones" sheetId="19" r:id="rId8"/>
+    <sheet name="Grades" sheetId="16" r:id="rId4"/>
+    <sheet name="Areas" sheetId="6" r:id="rId5"/>
+    <sheet name="Temas" sheetId="13" r:id="rId6"/>
+    <sheet name="Secciones" sheetId="19" r:id="rId7"/>
+    <sheet name="Materias" sheetId="4" r:id="rId8"/>
     <sheet name="Grades_Sections" sheetId="20" r:id="rId9"/>
     <sheet name="Subjects_Grades" sheetId="21" r:id="rId10"/>
     <sheet name="Herramientas" sheetId="10" r:id="rId11"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="394">
   <si>
     <t>Académico_2</t>
   </si>
@@ -1058,30 +1058,15 @@
     <t>Preschool</t>
   </si>
   <si>
-    <t>K4,K5,TR</t>
-  </si>
-  <si>
     <t>Primary School</t>
   </si>
   <si>
-    <t>01,02,03,04,05</t>
-  </si>
-  <si>
     <t>Middle School</t>
   </si>
   <si>
-    <t>06,07,08</t>
-  </si>
-  <si>
     <t>High School</t>
   </si>
   <si>
-    <t>09,10,11</t>
-  </si>
-  <si>
-    <t>grades</t>
-  </si>
-  <si>
     <t>Matemáticas</t>
   </si>
   <si>
@@ -1245,6 +1230,9 @@
   </si>
   <si>
     <t>Proyectos</t>
+  </si>
+  <si>
+    <t>school_code</t>
   </si>
 </sst>
 </file>
@@ -1345,7 +1333,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -1856,13 +1844,63 @@
     <border>
       <left/>
       <right style="thin">
-        <color theme="8" tint="0.39997558519241921"/>
+        <color theme="1"/>
       </right>
-      <top style="thin">
-        <color theme="8" tint="0.39997558519241921"/>
-      </top>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color theme="8" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1926,11 +1964,11 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1969,21 +2007,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2005,19 +2028,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="none">
-          <fgColor auto="1"/>
-          <bgColor auto="1"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2096,20 +2135,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor auto="1"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2125,7 +2163,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEEFDD8F-4E37-3C44-8405-6C28F806F3E5}" name="Table5" displayName="Table5" ref="A1:C39" insertRowShift="1" totalsRowShown="0" headerRowDxfId="4" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEEFDD8F-4E37-3C44-8405-6C28F806F3E5}" name="Table5" displayName="Table5" ref="A1:C39" insertRowShift="1" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{777CC35A-210A-B142-A229-D2FBB9E0942B}" name="grado" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{779C5F15-25C2-7F44-8D5A-CDA76703820A}" name="seccion" dataDxfId="2"/>
@@ -2501,8 +2539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9BC5D3F-1904-3B48-A5BA-62F71519D7B5}">
   <dimension ref="A1:B164"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7843,10 +7881,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AB04F78-20E6-F04A-A4CC-59D1F05547D5}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7854,10 +7892,9 @@
     <col min="1" max="1" width="18.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="2"/>
-    <col min="4" max="4" width="10.83203125" style="59"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
         <v>64</v>
       </c>
@@ -7867,11 +7904,8 @@
       <c r="C1" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="56" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
         <v>103</v>
       </c>
@@ -7881,50 +7915,38 @@
       <c r="C2" s="53">
         <v>40</v>
       </c>
-      <c r="D2" s="57" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="54" t="s">
         <v>104</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C3" s="55">
         <v>41</v>
       </c>
-      <c r="D3" s="58" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="52" t="s">
         <v>105</v>
       </c>
       <c r="B4" s="53" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C4" s="53">
         <v>42</v>
       </c>
-      <c r="D4" s="57" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="54" t="s">
         <v>106</v>
       </c>
       <c r="B5" s="55" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C5" s="55">
         <v>43</v>
-      </c>
-      <c r="D5" s="58" t="s">
-        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -7934,6 +7956,190 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20AB50A6-431D-184F-94EE-B7A1F485BCE2}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="63" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="63" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="64">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="55">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="55">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="55">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="55">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="56" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="56" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="53">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="53">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="56" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="56" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="53">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="56" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="56" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="55">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="56" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="56" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" s="55">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="56" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="56" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" s="55">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="57" t="s">
+        <v>168</v>
+      </c>
+      <c r="B13" s="57" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="53">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="53">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="57" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" s="57" t="s">
+        <v>170</v>
+      </c>
+      <c r="C15" s="53">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A6C17D-B7EE-4711-94AF-14518E98A3F5}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -7960,7 +8166,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B2" s="41" t="s">
         <v>108</v>
@@ -7985,7 +8191,7 @@
         <v>110</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="C4" s="41">
         <v>188</v>
@@ -7993,10 +8199,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C5" s="41">
         <v>189</v>
@@ -8007,7 +8213,7 @@
         <v>111</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C6" s="41">
         <v>190</v>
@@ -8029,7 +8235,7 @@
         <v>113</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C8" s="41">
         <v>192</v>
@@ -8037,10 +8243,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C9" s="41">
         <v>193</v>
@@ -8048,7 +8254,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="41" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B10" s="41" t="s">
         <v>152</v>
@@ -8062,7 +8268,7 @@
         <v>114</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C11" s="41">
         <v>202</v>
@@ -8070,10 +8276,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="41" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C12" s="41">
         <v>195</v>
@@ -8084,7 +8290,7 @@
         <v>115</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="C13" s="41">
         <v>196</v>
@@ -8092,7 +8298,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="41" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="B14" s="41" t="s">
         <v>158</v>
@@ -8106,7 +8312,7 @@
         <v>116</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="C15" s="41">
         <v>201</v>
@@ -8114,7 +8320,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="41" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B16" s="41" t="s">
         <v>117</v>
@@ -8125,10 +8331,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="41" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="C17" s="41">
         <v>199</v>
@@ -8140,7 +8346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13288D26-1715-43A0-91D2-35D274861EBC}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -8223,137 +8429,46 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20AB50A6-431D-184F-94EE-B7A1F485BCE2}">
-  <dimension ref="A1:B15"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB9281A-B767-3444-947F-A4BE344A4582}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="10.83203125" style="2"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="37" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="61" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="61" t="s">
-        <v>127</v>
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="61" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="61" t="s">
-        <v>128</v>
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="61" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="61" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="61" t="s">
-        <v>130</v>
-      </c>
-      <c r="B5" s="61" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="61" t="s">
-        <v>131</v>
-      </c>
-      <c r="B6" s="61" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="61" t="s">
-        <v>132</v>
-      </c>
-      <c r="B7" s="61" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="61" t="s">
-        <v>133</v>
-      </c>
-      <c r="B8" s="61" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="61" t="s">
-        <v>134</v>
-      </c>
-      <c r="B9" s="61" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="61" t="s">
-        <v>135</v>
-      </c>
-      <c r="B10" s="61" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="61" t="s">
-        <v>136</v>
-      </c>
-      <c r="B11" s="61" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="61" t="s">
-        <v>137</v>
-      </c>
-      <c r="B12" s="61" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="62" t="s">
-        <v>168</v>
-      </c>
-      <c r="B13" s="62" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="63" t="s">
-        <v>169</v>
-      </c>
-      <c r="B14" s="63" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="62" t="s">
-        <v>170</v>
-      </c>
-      <c r="B15" s="62" t="s">
-        <v>170</v>
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -8362,11 +8477,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81DEEA14-CFFA-4C60-B0C0-920B78619759}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -8393,71 +8508,71 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="64">
+      <c r="C2" s="59">
         <v>849</v>
       </c>
-      <c r="D2" s="66">
+      <c r="D2" s="61">
         <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="64">
+      <c r="C3" s="59">
         <v>850</v>
       </c>
-      <c r="D3" s="66">
+      <c r="D3" s="61">
         <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="C4" s="64">
+      <c r="C4" s="59">
         <v>853</v>
       </c>
-      <c r="D4" s="66">
+      <c r="D4" s="61">
         <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="C5" s="64">
+        <v>359</v>
+      </c>
+      <c r="C5" s="59">
         <v>852</v>
       </c>
-      <c r="D5" s="66">
+      <c r="D5" s="61">
         <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="C6" s="64">
+        <v>361</v>
+      </c>
+      <c r="C6" s="59">
         <v>851</v>
       </c>
-      <c r="D6" s="66">
+      <c r="D6" s="61">
         <v>187</v>
       </c>
     </row>
@@ -8466,54 +8581,54 @@
         <v>143</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="C7" s="64">
+        <v>362</v>
+      </c>
+      <c r="C7" s="59">
         <v>855</v>
       </c>
-      <c r="D7" s="66">
+      <c r="D7" s="61">
         <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="C8" s="64">
+        <v>339</v>
+      </c>
+      <c r="C8" s="59">
         <v>854</v>
       </c>
-      <c r="D8" s="66">
+      <c r="D8" s="61">
         <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="C9" s="64">
+        <v>365</v>
+      </c>
+      <c r="C9" s="59">
         <v>856</v>
       </c>
-      <c r="D9" s="66">
+      <c r="D9" s="61">
         <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="C10" s="64">
+        <v>341</v>
+      </c>
+      <c r="C10" s="59">
         <v>857</v>
       </c>
-      <c r="D10" s="66">
+      <c r="D10" s="61">
         <v>189</v>
       </c>
     </row>
@@ -8522,12 +8637,12 @@
         <v>146</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="C11" s="64">
+        <v>342</v>
+      </c>
+      <c r="C11" s="59">
         <v>858</v>
       </c>
-      <c r="D11" s="66">
+      <c r="D11" s="61">
         <v>190</v>
       </c>
     </row>
@@ -8536,138 +8651,138 @@
         <v>147</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="C12" s="64">
+        <v>367</v>
+      </c>
+      <c r="C12" s="59">
         <v>859</v>
       </c>
-      <c r="D12" s="66">
+      <c r="D12" s="61">
         <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="C13" s="64">
+      <c r="C13" s="59">
         <v>861</v>
       </c>
-      <c r="D13" s="66">
+      <c r="D13" s="61">
         <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C14" s="64">
+      <c r="C14" s="59">
         <v>860</v>
       </c>
-      <c r="D14" s="66">
+      <c r="D14" s="61">
         <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>348</v>
-      </c>
-      <c r="C15" s="64">
+        <v>343</v>
+      </c>
+      <c r="C15" s="59">
         <v>862</v>
       </c>
-      <c r="D15" s="66">
+      <c r="D15" s="61">
         <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>350</v>
-      </c>
-      <c r="C16" s="64">
+        <v>345</v>
+      </c>
+      <c r="C16" s="59">
         <v>863</v>
       </c>
-      <c r="D16" s="66">
+      <c r="D16" s="61">
         <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C17" s="64">
+      <c r="C17" s="59">
         <v>867</v>
       </c>
-      <c r="D17" s="66">
+      <c r="D17" s="61">
         <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="C18" s="64">
+        <v>374</v>
+      </c>
+      <c r="C18" s="59">
         <v>865</v>
       </c>
-      <c r="D18" s="66">
+      <c r="D18" s="61">
         <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>381</v>
-      </c>
-      <c r="C19" s="64">
+        <v>376</v>
+      </c>
+      <c r="C19" s="59">
         <v>866</v>
       </c>
-      <c r="D19" s="66">
+      <c r="D19" s="61">
         <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="C20" s="64">
+        <v>378</v>
+      </c>
+      <c r="C20" s="59">
         <v>887</v>
       </c>
-      <c r="D20" s="66">
+      <c r="D20" s="61">
         <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>354</v>
-      </c>
-      <c r="C21" s="64">
+        <v>349</v>
+      </c>
+      <c r="C21" s="59">
         <v>868</v>
       </c>
-      <c r="D21" s="66">
+      <c r="D21" s="61">
         <v>195</v>
       </c>
     </row>
@@ -8676,12 +8791,12 @@
         <v>157</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="C22" s="64">
+        <v>350</v>
+      </c>
+      <c r="C22" s="59">
         <v>869</v>
       </c>
-      <c r="D22" s="66">
+      <c r="D22" s="61">
         <v>196</v>
       </c>
     </row>
@@ -8690,96 +8805,96 @@
         <v>158</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="C23" s="64">
+        <v>379</v>
+      </c>
+      <c r="C23" s="59">
         <v>870</v>
       </c>
-      <c r="D23" s="66">
+      <c r="D23" s="61">
         <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C24" s="64">
+      <c r="C24" s="59">
         <v>871</v>
       </c>
-      <c r="D24" s="66">
+      <c r="D24" s="61">
         <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="C25" s="64">
+        <v>382</v>
+      </c>
+      <c r="C25" s="59">
         <v>894</v>
       </c>
-      <c r="D25" s="66">
+      <c r="D25" s="61">
         <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="C26" s="64">
+        <v>384</v>
+      </c>
+      <c r="C26" s="59">
         <v>873</v>
       </c>
-      <c r="D26" s="66">
+      <c r="D26" s="61">
         <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>390</v>
-      </c>
-      <c r="C27" s="64">
+        <v>385</v>
+      </c>
+      <c r="C27" s="59">
         <v>891</v>
       </c>
-      <c r="D27" s="66">
+      <c r="D27" s="61">
         <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="C28" s="64">
+        <v>387</v>
+      </c>
+      <c r="C28" s="59">
         <v>892</v>
       </c>
-      <c r="D28" s="66">
+      <c r="D28" s="61">
         <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>394</v>
-      </c>
-      <c r="C29" s="64">
+        <v>389</v>
+      </c>
+      <c r="C29" s="59">
         <v>893</v>
       </c>
-      <c r="D29" s="66">
+      <c r="D29" s="61">
         <v>199</v>
       </c>
     </row>
@@ -8788,12 +8903,12 @@
         <v>159</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="C30" s="64">
+        <v>390</v>
+      </c>
+      <c r="C30" s="59">
         <v>881</v>
       </c>
-      <c r="D30" s="66">
+      <c r="D30" s="61">
         <v>201</v>
       </c>
     </row>
@@ -8804,100 +8919,52 @@
       <c r="B31" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C31" s="64">
+      <c r="C31" s="59">
         <v>882</v>
       </c>
-      <c r="D31" s="66">
+      <c r="D31" s="61">
         <v>201</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C32" s="64">
+      <c r="C32" s="59">
         <v>884</v>
       </c>
-      <c r="D32" s="66">
+      <c r="D32" s="61">
         <v>201</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="C33" s="65">
+        <v>347</v>
+      </c>
+      <c r="C33" s="60">
         <v>883</v>
       </c>
-      <c r="D33" s="67">
+      <c r="D33" s="62">
         <v>202</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="67"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="62"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C2:C33">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB9281A-B767-3444-947F-A4BE344A4582}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
se avanza en el front para el formulario Tipo Explora
</commit_message>
<xml_diff>
--- a/backend/data/DataWise_data.xlsx
+++ b/backend/data/DataWise_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/Documents/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8734020-8694-D948-BBA3-AEFE5B1F2A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6244E311-438F-104A-AA50-C396BAB940DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="580" windowWidth="42820" windowHeight="12360" firstSheet="2" activeTab="8" xr2:uid="{44AB9135-6F36-43A2-8618-128F6D28EF18}"/>
+    <workbookView xWindow="5040" yWindow="4580" windowWidth="36420" windowHeight="19960" activeTab="12" xr2:uid="{44AB9135-6F36-43A2-8618-128F6D28EF18}"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="18" r:id="rId1"/>
@@ -2590,30 +2590,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDotDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDotDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDotDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDotDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -2741,16 +2718,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2840,6 +2807,16 @@
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2854,11 +2831,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEEFDD8F-4E37-3C44-8405-6C28F806F3E5}" name="Table5" displayName="Table5" ref="A1:C39" insertRowShift="1" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEEFDD8F-4E37-3C44-8405-6C28F806F3E5}" name="Table5" displayName="Table5" ref="A1:C39" insertRowShift="1" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{777CC35A-210A-B142-A229-D2FBB9E0942B}" name="grado" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{779C5F15-25C2-7F44-8D5A-CDA76703820A}" name="seccion" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{01C133AA-140E-F045-A6F4-FB94327B8A12}" name="code" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{777CC35A-210A-B142-A229-D2FBB9E0942B}" name="grado" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{779C5F15-25C2-7F44-8D5A-CDA76703820A}" name="seccion" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{01C133AA-140E-F045-A6F4-FB94327B8A12}" name="code" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3163,8 +3140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AAD4E0-7EF2-134F-A9A0-0DE4803FFE3F}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3230,8 +3207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9BC5D3F-1904-3B48-A5BA-62F71519D7B5}">
   <dimension ref="A1:B164"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4561,8 +4538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC971763-5D00-4250-9727-92AE8EE7AF1D}">
   <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A43" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6350,15 +6327,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{286B85C5-CA1D-420C-A0D3-E35991CBC120}">
   <dimension ref="A1:D697"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C699" sqref="C699"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -16123,7 +16100,7 @@
   <autoFilter ref="A1:D697" xr:uid="{286B85C5-CA1D-420C-A0D3-E35991CBC120}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D1:D697">
-    <cfRule type="containsText" dxfId="6" priority="1" stopIfTrue="1" operator="containsText" text="power e">
+    <cfRule type="containsText" dxfId="5" priority="1" stopIfTrue="1" operator="containsText" text="power e">
       <formula>NOT(ISERROR(SEARCH("power e",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16135,14 +16112,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F276F6-33EA-40C9-B929-6DEBAF0DDEAA}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A25"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.33203125" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.83203125" bestFit="1" customWidth="1"/>
@@ -16199,7 +16176,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="56" t="s">
         <v>612</v>
       </c>
@@ -16216,7 +16193,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="56" t="s">
         <v>613</v>
       </c>
@@ -16233,7 +16210,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="56" t="s">
         <v>614</v>
       </c>
@@ -16248,7 +16225,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="57" t="s">
         <v>584</v>
       </c>
@@ -16299,7 +16276,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="56" t="s">
         <v>589</v>
       </c>
@@ -16367,7 +16344,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="56" t="s">
         <v>615</v>
       </c>
@@ -16416,7 +16393,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="56" t="s">
         <v>482</v>
       </c>
@@ -16450,7 +16427,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="56" t="s">
         <v>618</v>
       </c>
@@ -16463,7 +16440,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="56" t="s">
         <v>619</v>
       </c>
@@ -16506,7 +16483,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A23" s="56" t="s">
         <v>622</v>
       </c>
@@ -16556,7 +16533,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B1:E1">
-    <cfRule type="containsBlanks" dxfId="5" priority="3">
+    <cfRule type="containsBlanks" dxfId="4" priority="3">
       <formula>LEN(TRIM(B1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17656,10 +17633,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392E348C-14A0-4F43-A248-CDFC09B373D7}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17744,7 +17724,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17820,7 +17800,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18004,7 +17984,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18208,10 +18188,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13288D26-1715-43A0-91D2-35D274861EBC}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18294,7 +18277,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18341,8 +18324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81DEEA14-CFFA-4C60-B0C0-920B78619759}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18817,7 +18800,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C2:C33">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18827,7 +18810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FD6D4A-A47C-1C4C-8803-499599698761}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adds news fields to IRA_Questions (short _question, help, acronym), modify model, seeder , in front, displays help field
compiles to prod
</commit_message>
<xml_diff>
--- a/backend/data/DataWise_data.xlsx
+++ b/backend/data/DataWise_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/Documents/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4E8A45-633C-184B-B451-C69965E77391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8693FE90-7AE5-0446-BA37-B3BEF47C2EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18440" yWindow="5460" windowWidth="33040" windowHeight="17140" firstSheet="3" activeTab="14" xr2:uid="{DC49BAA6-999A-4FE5-B779-169158BBC25B}"/>
+    <workbookView xWindow="23200" yWindow="8120" windowWidth="26920" windowHeight="13360" firstSheet="7" activeTab="14" xr2:uid="{DC49BAA6-999A-4FE5-B779-169158BBC25B}"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="119">
   <si>
     <t>name_es</t>
   </si>
@@ -393,6 +393,9 @@
   </si>
   <si>
     <t>Consultas</t>
+  </si>
+  <si>
+    <t>Generación de informes</t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E14098-8805-41B2-8C67-DC3BA56DD845}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A35" sqref="A35:XFD45"/>
     </sheetView>
   </sheetViews>
@@ -1553,7 +1556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F48E7AE-E70B-486E-847A-A15402EC1EFE}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A35" sqref="A35:XFD50"/>
     </sheetView>
   </sheetViews>
@@ -2234,10 +2237,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2255903-7448-4E02-B0E5-6BA806B31308}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2405,6 +2408,14 @@
         <v>102</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2415,7 +2426,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2424,7 +2435,7 @@
     <col min="2" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -2462,6 +2473,9 @@
       </c>
       <c r="E2" t="s">
         <v>117</v>
+      </c>
+      <c r="F2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
cambia tamaño boton FormStatusBar dinamicamente cuando se hace click en este
</commit_message>
<xml_diff>
--- a/backend/data/DataWise_data.xlsx
+++ b/backend/data/DataWise_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ingrid.valero\OneDrive - FINAC S.A.S\Documents\Formularios_OIHUB\DOMECQ\Plantillas_oficiales_cargue_DOMECQ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0DCBD3-235A-4324-86E9-4F3786EBC8B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F3A62F-242D-D741-8C98-C459D8AC9756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" firstSheet="9" activeTab="14" xr2:uid="{C0404901-9F80-43D7-8D27-DC63BDCF4936}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12340" activeTab="5" xr2:uid="{C0404901-9F80-43D7-8D27-DC63BDCF4936}"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="1" r:id="rId1"/>
@@ -264,25 +264,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -325,9 +320,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -365,7 +360,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -471,7 +466,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -613,7 +608,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -623,24 +618,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2600D17-FF0E-42D3-BB76-E87F182BFB15}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -648,7 +643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -656,7 +651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -664,7 +659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -672,7 +667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -680,7 +675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -688,7 +683,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -696,7 +691,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -704,7 +699,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -712,7 +707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -720,7 +715,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -742,21 +737,21 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
     </row>
@@ -773,16 +768,16 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -802,7 +797,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -810,7 +805,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -818,7 +813,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -839,15 +834,15 @@
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -861,36 +856,36 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -907,12 +902,12 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="33.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -929,190 +924,190 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>43</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>44</v>
       </c>
       <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>45</v>
       </c>
       <c r="B8" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>46</v>
       </c>
       <c r="B9" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>47</v>
       </c>
       <c r="B10" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>48</v>
       </c>
       <c r="B11" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>54</v>
       </c>
       <c r="B12" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="C12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1134,9 +1129,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1153,17 +1148,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2963BAE1-A0F6-44F0-BCA5-184B22FCA16A}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -1177,57 +1172,57 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1245,9 +1240,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1258,7 +1253,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1282,9 +1277,9 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1295,7 +1290,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1319,9 +1314,9 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1332,7 +1327,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1356,12 +1351,12 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1372,7 +1367,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1383,7 +1378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1394,7 +1389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1405,7 +1400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1416,7 +1411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1427,7 +1422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1438,7 +1433,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1449,7 +1444,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1460,7 +1455,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1471,7 +1466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1482,7 +1477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1502,13 +1497,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC577E22-40D0-43E6-B799-651572071037}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1516,7 +1511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1537,9 +1532,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1547,7 +1542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1568,12 +1563,12 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1587,7 +1582,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1601,7 +1596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1615,7 +1610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1629,7 +1624,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1643,7 +1638,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1657,7 +1652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1671,7 +1666,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1685,7 +1680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1699,7 +1694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1713,7 +1708,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1727,7 +1722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1754,9 +1749,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1767,7 +1762,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>

</xml_diff>